<commit_message>
Generating OWL file for initial dataset of entries
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B577292C-B401-BE46-9DB8-B034F7D9BF23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED99C07-8507-B04C-BE7B-4312CB53B616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="-13860" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15220" yWindow="-13880" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>http://purl.obolibrary.org/obo/mf.owl</t>
   </si>
   <si>
-    <t>has output [RO:0002234]; realizes [BFO:0000055]; realized in [BFO:0000054]; output of [RO:0002353]</t>
-  </si>
-  <si>
     <t xml:space="preserve">has occurrent part [BFO:0000117]; has profile [BFO:0000119] </t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>http://purl.obolibrary.org/obo/omrse.owl</t>
   </si>
   <si>
-    <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]</t>
-  </si>
-  <si>
     <t>BCIO</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>biological role [CHEBI:24432]</t>
   </si>
   <si>
-    <t>Carcinogen [CHEBI:50903];Alcohol dehydrogenase 1B [CHEBI:50269]</t>
-  </si>
-  <si>
     <t>﻿Antidepressant drug [CHEBI:35469];Antimanic drug [CHEBI:35477];Antipsychotic drug [CHEBI:35476];Anxiolytic drug [CHEBI:35474];Central nervous system depressent [CHEBI:35488];Central nervous system drug [CHEBI:35470];Pharmaceutical [CHEBI:52217];Tranquilizing drug  [CHEBI:35473];Drug [CHEBI:23888]</t>
   </si>
   <si>
@@ -274,6 +265,15 @@
   </si>
   <si>
     <t>Anatomical system [UBERON:0000467]; Death [UBERON:035944]; Organ [UBERON:0000062]; Life cycle temporal boundary [UBERON:0035943]</t>
+  </si>
+  <si>
+    <t>Carcinogen [CHEBI:50903];Alcohol dehydrogenase 1B [CHEBI:50269]; Flavouring agent [CHEBI:35617]</t>
+  </si>
+  <si>
+    <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]; derives from [RO:0001000]; has role [RO:0000087]</t>
+  </si>
+  <si>
+    <t>has output [RO:0002234]; realizes [BFO:0000055]; realized in [BFO:0000054]; output of [RO:0002353]; contains [RO:0001019]</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,92 +676,92 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -775,10 +775,10 @@
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -792,44 +792,44 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -843,64 +843,64 @@
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -911,13 +911,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -928,10 +928,10 @@
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -945,10 +945,10 @@
         <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -962,10 +962,10 @@
         <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -996,61 +996,61 @@
         <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates (fixing parents etc.)
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60C81A2-820D-8B46-8A1C-AD1AA12234F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB5790F-E75D-2C47-9B4D-AD735E207928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5380" yWindow="1820" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>planned process [OBI:0000011]</t>
   </si>
   <si>
-    <t>is about [IAO:0000136]; data item [IAO:0000027]; report [IAO:0000088]; plan specification [IAO:0000104]</t>
-  </si>
-  <si>
     <t>SEPIO</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>planned process [OBI:0000011]; organisation [OBI:0000245]; dose [OBI:0000984]</t>
   </si>
   <si>
-    <t>Credible interval [OBCS:0000071]; Mortality ratio [OBCS:0000150]</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/uberon.owl</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>http://purl.obolibrary.org/obo/po.owl</t>
   </si>
   <si>
-    <t>whole plant [PO:0005679]</t>
-  </si>
-  <si>
     <t>pharmaceutical [CHEBI:52217]</t>
   </si>
   <si>
@@ -240,9 +231,6 @@
     <t>injury [OGMS:0000102]</t>
   </si>
   <si>
-    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO_0000029]; occurrent [BFO_0000003]</t>
-  </si>
-  <si>
     <t>MFOEM</t>
   </si>
   <si>
@@ -289,6 +277,18 @@
   </si>
   <si>
     <t>Individual human behaviour [BCIO:036000]; Individual human activity [BCIO:040000]; Population behaviour [BCIO:034000]; Human behaviour [BCIO:042000]; Intervention evaluation [BCIO:038000]; Process attribute [BCIO:043000]</t>
+  </si>
+  <si>
+    <t>whole plant [PO:0000003]</t>
+  </si>
+  <si>
+    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; occurrent [BFO:0000003]; process boundary [BFO:0000035]</t>
+  </si>
+  <si>
+    <t>is about [IAO:0000136]; data item [IAO:0000027]; report [IAO:0000088]; plan specification [IAO:0000104]; material information bearer [IAO:0000178]; document [IAO:0000310]</t>
+  </si>
+  <si>
+    <t>Credible interval [OBCS:0000071]; Mortality ratio [OBCS:0000150]; model [OBCS:0000035]</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,172 +692,172 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -868,81 +868,81 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -953,13 +953,13 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -970,13 +970,13 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -987,16 +987,16 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1004,16 +1004,16 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1021,81 +1021,81 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up for rebuild
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627802BC-2AE6-FF46-BD30-4CBBCF9DA01E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA559490-F647-4246-ABE4-619FE723F5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5380" yWindow="1800" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>whole plant [PO:0000003]</t>
   </si>
   <si>
-    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; occurrent [BFO:0000003]; process boundary [BFO:0000035]</t>
-  </si>
-  <si>
     <t>Credible interval [OBCS:0000071]; Mortality ratio [OBCS:0000150]; model [OBCS:0000035]</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>chromatography [CHMO:0001000]; liquid chromatography [CHMO:0001004]</t>
+  </si>
+  <si>
+    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; occurrent [BFO:0000003]; process boundary [BFO:0000035]; temporal region [BFO:0000008]</t>
   </si>
 </sst>
 </file>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>44</v>
@@ -747,7 +747,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>44</v>
@@ -764,7 +764,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
@@ -985,7 +985,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>45</v>
@@ -1019,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>44</v>
@@ -1036,7 +1036,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>44</v>
@@ -1112,16 +1112,16 @@
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Add extra imported entries
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460C3DDA-029D-8F45-B8A7-B92350F9F4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906F79DD-BD57-3E45-8822-55835B8B64F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="-16620" windowWidth="19940" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5200" yWindow="-17840" windowWidth="19940" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -180,9 +180,6 @@
     <t>biological role [CHEBI:24432]</t>
   </si>
   <si>
-    <t>﻿Antidepressant drug [CHEBI:35469];Antimanic drug [CHEBI:35477];Antipsychotic drug [CHEBI:35476];Anxiolytic drug [CHEBI:35474];Central nervous system depressent [CHEBI:35488];Central nervous system drug [CHEBI:35470];Pharmaceutical [CHEBI:52217];Tranquilizing drug  [CHEBI:35473];Drug [CHEBI:23888]</t>
-  </si>
-  <si>
     <t>CHEBI-DRUG-ROLE</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>http://purl.obolibrary.org/obo/mfoem.owl</t>
   </si>
   <si>
-    <t>Carcinogen [CHEBI:50903];Alcohol dehydrogenase 1B [CHEBI:50269]; Flavouring agent [CHEBI:35617]</t>
-  </si>
-  <si>
     <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]; derives from [RO:0001000]; has role [RO:0000087]</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>has output [RO:0002234]; realizes [BFO:0000055]; realized in [BFO:0000054]; output of [RO:0002353]; contains [RO:0001019]; system [RO:0002577]</t>
   </si>
   <si>
-    <t>Amphetamine [CHEBI:2679];Baclofen [CHEBI:2972];Benzodiazepine [CHEBI:22720];Buprenorphine [CHEBI:3216];Bupropion [CHEBI:3219];Caffeine [CHEBI:27732];Cannabinoid [CHEBI:67194];Chemical substance [CHEBI:59999];Cocaine [CHEBI:27958];Codeine [CHEBI:38164];Ethanol [CHEBI:16236];Fentanyl [CHEBI:119915];Formaldehyde [CHEBI:16842];Gabapentin [CHEBI:42797];Heroin [CHEBI:27808];Methadone [CHEBI:6807];Methadrone  [CHEBI:59331];Methamphetamine [CHEBI:6809];Naloxone [CHEBI:7459];Nicotine [CHEBI:18723];4-(N-nitrosomethylamino)-1-(3-pyridyl)butan-1-one [CHEBI:32692];Synthetic cannabinoid [CHEBI:67201];Tetrahydrocannabinol [CHEBI:66964];Varenicline [CHEBI:84500]; nitrosamine [CHEBI:35803]</t>
-  </si>
-  <si>
     <t>CHMO</t>
   </si>
   <si>
@@ -301,6 +292,24 @@
   </si>
   <si>
     <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; occurrent [BFO:0000003]; process boundary [BFO:0000035]; temporal region [BFO:0000008]; fiat object part [﻿BFO:0000024]; immaterial entity [BFO:0000141]</t>
+  </si>
+  <si>
+    <t>﻿Antidepressant drug [CHEBI:35469];Antimanic drug [CHEBI:35477];Antipsychotic drug [CHEBI:35476];Anxiolytic drug [CHEBI:35474];Central nervous system depressent [CHEBI:35488];Central nervous system drug [CHEBI:35470];Pharmaceutical [CHEBI:52217];Tranquilizing drug  [CHEBI:35473];Drug [CHEBI:23888]; psychotropic drug [CHEBI:35471]; opioid analgesic [CHEBI:35482]</t>
+  </si>
+  <si>
+    <t>Carcinogen [CHEBI:50903];Alcohol dehydrogenase 1B [CHEBI:50269]; Flavouring agent [CHEBI:35617]; nicotinic acetylcholine receptor agonist [CHEBI:47958]; nicotinic antagonist [CHEBI:48878]; carcinogenic agent [CHEBI:50903]; cannabinoid receptor agonist [CHEBI:67072]; cb1 receptor antagonist [CHEBI:73416]; cb2 receptor agonist [CHEBI:73417]</t>
+  </si>
+  <si>
+    <t>ERO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ero.owl</t>
+  </si>
+  <si>
+    <t>intubation [ERO:0001108]</t>
+  </si>
+  <si>
+    <t>Amphetamine [CHEBI:2679];Baclofen [CHEBI:2972];Benzodiazepine [CHEBI:22720];Buprenorphine [CHEBI:3216];Bupropion [CHEBI:3219];Caffeine [CHEBI:27732];Cannabinoid [CHEBI:67194];Chemical substance [CHEBI:59999];Cocaine [CHEBI:27958];Codeine [CHEBI:38164];Ethanol [CHEBI:16236];Fentanyl [CHEBI:119915];Formaldehyde [CHEBI:16842];Gabapentin [CHEBI:42797];Heroin [CHEBI:27808];Methadone [CHEBI:6807];Methadrone  [CHEBI:59331];Methamphetamine [CHEBI:6809];Naloxone [CHEBI:7459];Nicotine [CHEBI:18723];4-(N-nitrosomethylamino)-1-(3-pyridyl)butan-1-one [CHEBI:32692];Synthetic cannabinoid [CHEBI:67201];Tetrahydrocannabinol [CHEBI:66964];Varenicline [CHEBI:84500];nitrosamine [CHEBI:35803]; Atomoxetine [CHEBI:127342];naphthalene [CHEBI:16482];propanal [CHEBI:17153];carbon monoxide [CHEBI:17245]; nicotine [CHEBI:18723]; carbonyl compound [CHEBI:36586]; elemental cadmium [CHEBI:37249]; pyrene [CHEBI:39106]; cytisine [CHEBI:4055]; crotonaldehyde [CHEBI:41607]; diazepam [CHEBI:49575]; hydrocodone [CHEBI:5779]; cannabidiol [CHEBI:69478]; oxycodone [CHEBI:7852]; rimonabant [CHEBI:34967]</t>
   </si>
 </sst>
 </file>
@@ -681,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,7 +722,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -721,19 +730,19 @@
         <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -747,13 +756,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="372" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>46</v>
       </c>
@@ -764,13 +773,13 @@
         <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -781,24 +790,24 @@
         <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>45</v>
@@ -840,16 +849,16 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>45</v>
@@ -908,16 +917,16 @@
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>44</v>
@@ -925,16 +934,16 @@
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
       <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>44</v>
@@ -948,7 +957,7 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>42</v>
@@ -968,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>45</v>
@@ -985,7 +994,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>45</v>
@@ -1019,7 +1028,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>44</v>
@@ -1036,7 +1045,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>44</v>
@@ -1053,7 +1062,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>44</v>
@@ -1061,16 +1070,16 @@
     </row>
     <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>44</v>
@@ -1078,16 +1087,16 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>44</v>
@@ -1095,16 +1104,16 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>44</v>
@@ -1112,19 +1121,36 @@
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="E25" s="5" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert labels to lower case
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906F79DD-BD57-3E45-8822-55835B8B64F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3526F154-DBD2-8E48-B524-DF0A1CB064E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="-17840" windowWidth="19940" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; occurrent [BFO:0000003]; process boundary [BFO:0000035]; temporal region [BFO:0000008]; fiat object part [﻿BFO:0000024]; immaterial entity [BFO:0000141]</t>
   </si>
   <si>
-    <t>﻿Antidepressant drug [CHEBI:35469];Antimanic drug [CHEBI:35477];Antipsychotic drug [CHEBI:35476];Anxiolytic drug [CHEBI:35474];Central nervous system depressent [CHEBI:35488];Central nervous system drug [CHEBI:35470];Pharmaceutical [CHEBI:52217];Tranquilizing drug  [CHEBI:35473];Drug [CHEBI:23888]; psychotropic drug [CHEBI:35471]; opioid analgesic [CHEBI:35482]</t>
-  </si>
-  <si>
     <t>Carcinogen [CHEBI:50903];Alcohol dehydrogenase 1B [CHEBI:50269]; Flavouring agent [CHEBI:35617]; nicotinic acetylcholine receptor agonist [CHEBI:47958]; nicotinic antagonist [CHEBI:48878]; carcinogenic agent [CHEBI:50903]; cannabinoid receptor agonist [CHEBI:67072]; cb1 receptor antagonist [CHEBI:73416]; cb2 receptor agonist [CHEBI:73417]</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>Amphetamine [CHEBI:2679];Baclofen [CHEBI:2972];Benzodiazepine [CHEBI:22720];Buprenorphine [CHEBI:3216];Bupropion [CHEBI:3219];Caffeine [CHEBI:27732];Cannabinoid [CHEBI:67194];Chemical substance [CHEBI:59999];Cocaine [CHEBI:27958];Codeine [CHEBI:38164];Ethanol [CHEBI:16236];Fentanyl [CHEBI:119915];Formaldehyde [CHEBI:16842];Gabapentin [CHEBI:42797];Heroin [CHEBI:27808];Methadone [CHEBI:6807];Methadrone  [CHEBI:59331];Methamphetamine [CHEBI:6809];Naloxone [CHEBI:7459];Nicotine [CHEBI:18723];4-(N-nitrosomethylamino)-1-(3-pyridyl)butan-1-one [CHEBI:32692];Synthetic cannabinoid [CHEBI:67201];Tetrahydrocannabinol [CHEBI:66964];Varenicline [CHEBI:84500];nitrosamine [CHEBI:35803]; Atomoxetine [CHEBI:127342];naphthalene [CHEBI:16482];propanal [CHEBI:17153];carbon monoxide [CHEBI:17245]; nicotine [CHEBI:18723]; carbonyl compound [CHEBI:36586]; elemental cadmium [CHEBI:37249]; pyrene [CHEBI:39106]; cytisine [CHEBI:4055]; crotonaldehyde [CHEBI:41607]; diazepam [CHEBI:49575]; hydrocodone [CHEBI:5779]; cannabidiol [CHEBI:69478]; oxycodone [CHEBI:7852]; rimonabant [CHEBI:34967]</t>
+  </si>
+  <si>
+    <t>﻿Antidepressant drug [CHEBI:35469];Antimanic drug [CHEBI:35477];Antipsychotic drug [CHEBI:35476];Anxiolytic drug [CHEBI:35474];Central nervous system depressent [CHEBI:35488];Central nervous system drug [CHEBI:35470];Pharmaceutical [CHEBI:52217];Tranquilizing drug  [CHEBI:35473];Drug [CHEBI:23888]; psychotropic drug [CHEBI:35471]; opioid analgesic [CHEBI:35482]; antitussive [CHEBI:51177]</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +773,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
@@ -790,13 +790,13 @@
         <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -807,7 +807,7 @@
         <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>45</v>
@@ -1138,16 +1138,16 @@
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
         <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>84</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Removed HP & switched to CHEBI-lite
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1847FED2-9D3B-4975-9AF3-AE52EFB505DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0386E96-4427-D94E-9F05-C0240E2B70ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="28170" windowHeight="14040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="28180" windowHeight="14040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -88,9 +88,6 @@
     <t>CHEBI-BIO-ROLE</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/chebi.owl</t>
-  </si>
-  <si>
     <t>biological role [CHEBI:24432]</t>
   </si>
   <si>
@@ -304,15 +301,6 @@
     <t>Life cycle temporal boundary [UBERON:0035943]; death [UBERON:035944]; death stage [UBERON:0000071]</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/hp.owl</t>
-  </si>
-  <si>
-    <t>aortic stiffness [HP:0030965]</t>
-  </si>
-  <si>
     <t>GSSO</t>
   </si>
   <si>
@@ -326,13 +314,16 @@
   </si>
   <si>
     <t>outpatient role [BCIO:015080]; intervention [BCIO:037000]; personal life attribute [BCIO:050302]; human population [BCIO:041000]; subjective want [BCIO:050317]; consumption behaviour [BCIO:036061];  human age [BCIO:015015]; individual human behaviour [BCIO:036000]; highest level of formal educational qualification achieved [BCIO:015243]; homeless person [BCIO:015036]; ﻿personal role [BCIO:006081]; inpatient role [BCIO:015079]; individual human activity [BCIO:040000]; personal disposition [BCIO:050301]; personal attribute [BCIO:050300]; pleasure associated with a behaviour [BCIO:006159]; hospital outpatient facility [BCIO:026015]; personal quality [BCIO:050303]; prescribing behaviour [BCIO:050354]; population behaviour [BCIO:034000]; human behaviour [BCIO:042000]; bisexual [BCIO:015005]; within-country location [BCIO:026002]; e-cigarette use [BCIO:050377]; bodily process [OGMS:0000060]; object-using behaviour [BCIO:036027]</t>
+  </si>
+  <si>
+    <t>https://ftp.ebi.ac.uk/pub/databases/chebi/ontology/chebi_lite.owl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -666,21 +657,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:F1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.125" customWidth="1"/>
-    <col min="3" max="3" width="27.625" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -717,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="409.5" customHeight="1">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -728,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -737,7 +728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="117" customHeight="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -754,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -771,425 +762,408 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="86.25" customHeight="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="327" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="327" customHeight="1">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="117" customHeight="1">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="121.5" customHeight="1">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="250.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="250.5" customHeight="1">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="74.25" customHeight="1">
+    <row r="13" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29.25" customHeight="1">
+    <row r="17" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>58</v>
       </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>69</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.5" customHeight="1">
+    <row r="23" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="E23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="86.25" customHeight="1">
+    <row r="24" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" customHeight="1">
+    <row r="25" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
         <v>83</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>84</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>86</v>
       </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="86.25" customHeight="1">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>88</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>90</v>
       </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
         <v>91</v>
       </c>
-      <c r="B27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>93</v>
       </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>94</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>96</v>
-      </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Remove confusion about planned process and activity
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7eb46d052d0a8996/Documents/GitHub/addiction-ontology/imports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{B0386E96-4427-D94E-9F05-C0240E2B70ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAF41334-8C36-47BB-8644-F8662EC1B180}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5291D5-ED46-D14A-80D2-03660252F376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="740" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -259,9 +259,6 @@
     <t>http://purl.obolibrary.org/obo/sepio.owl</t>
   </si>
   <si>
-    <t>planned process [OBI:0000011]</t>
-  </si>
-  <si>
     <t>research activity [SEPIO:0000004];﻿research study [SEPIO:0000125]</t>
   </si>
   <si>
@@ -296,13 +293,16 @@
   </si>
   <si>
     <t>outpatient role [BCIO:015080]; intervention [BCIO:037000]; personal life attribute [BCIO:050302]; human population [BCIO:041000]; subjective want [BCIO:050317]; consumption behaviour [BCIO:036061];  human age [BCIO:015015]; individual human behaviour [BCIO:036000]; highest level of formal educational qualification achieved [BCIO:015243]; homeless person [BCIO:015036]; ﻿personal role [BCIO:006081]; inpatient role [BCIO:015079]; individual human activity [BCIO:040000]; personal disposition [BCIO:050301]; personal attribute [BCIO:050300]; pleasure associated with a behaviour [BCIO:006159]; hospital outpatient facility [BCIO:026015]; personal quality [BCIO:050303]; prescribing behaviour [BCIO:050354]; population behaviour [BCIO:034000]; human behaviour [BCIO:042000]; bisexual [BCIO:015005]; within-country location [BCIO:026002]; e-cigarette use [BCIO:050377]; bodily process [OGMS:0000060]; object-using behaviour [BCIO:036027]; uniform process aggregate [BCIO:050267]; individual human behaviour pattern [BCIO:036100]; consumption behaviour pattern [BCIO:050210]; substance use behaviour pattern [BCIO:050211]; tobacco use behaviour pattern [BCIO:036102]; tobacco smoking behaviour pattern [BCIO:036104]; cigarette smoking behaviour pattern [BCIO:036106]; substance use behaviour [BCIO:036113]; cigarette smoking behaviour [BCIO:036105]; tobacco smoking behaviour [BCIO:036103]; tobacco use behaviour [BCIO:036114]; alcohol consumption [BCIO:050376]</t>
+  </si>
+  <si>
+    <t>research activity [SEPIO:0000004]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -458,10 +458,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,20 +638,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1048573"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.125" customWidth="1"/>
-    <col min="3" max="3" width="27.625" customWidth="1"/>
-    <col min="4" max="4" width="81.375" customWidth="1"/>
-    <col min="5" max="5" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -692,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="409.5" customHeight="1">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -703,7 +699,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -712,7 +708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="117" customHeight="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -729,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="90" customHeight="1">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -746,12 +742,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="86.25" customHeight="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -763,30 +759,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="327" customHeight="1">
+    <row r="7" spans="1:6" ht="327" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="117" customHeight="1">
+    <row r="8" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -799,7 +795,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="29.25" customHeight="1">
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -816,7 +812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="129.75" customHeight="1">
+    <row r="10" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -833,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="250.5" customHeight="1">
+    <row r="11" spans="1:6" ht="250.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -850,7 +846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -867,7 +863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="74.25" customHeight="1">
+    <row r="13" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -884,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.5" customHeight="1">
+    <row r="14" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -901,7 +897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29.25" customHeight="1">
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -918,7 +914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29.25" customHeight="1">
+    <row r="16" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -936,7 +932,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="61.5" customHeight="1">
+    <row r="17" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -953,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="59.25" customHeight="1">
+    <row r="18" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -964,13 +960,13 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.5" customHeight="1">
+    <row r="19" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -987,7 +983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1004,7 +1000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1021,7 +1017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="43.5" customHeight="1">
+    <row r="22" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1038,7 +1034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="86.25" customHeight="1">
+    <row r="23" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1055,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="31.5" customHeight="1">
+    <row r="24" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1063,57 +1059,57 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>80</v>
       </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="86.25" customHeight="1">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>82</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>84</v>
       </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
         <v>85</v>
       </c>
-      <c r="B26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
+    <row r="1048566" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048567" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>